<commit_message>
Wykresy i nowy gotoweic
</commit_message>
<xml_diff>
--- a/wyniki/wyniki.xlsx
+++ b/wyniki/wyniki.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="16830" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="16830" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Czas przetwarzania" sheetId="3" r:id="rId3"/>
+    <sheet name="Prędkość przetwarzania" sheetId="5" r:id="rId4"/>
+    <sheet name="Stopień łączenia dostępów" sheetId="6" r:id="rId5"/>
+    <sheet name="Zajętość multiprocesora" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="blok8Rozmiar64" localSheetId="0">Sheet1!$C$27:$W$28</definedName>
@@ -276,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
   <si>
     <t>Rozmiar bloku</t>
   </si>
@@ -424,6 +427,21 @@
   <si>
     <t>DANE</t>
   </si>
+  <si>
+    <t>WERSJA 5</t>
+  </si>
+  <si>
+    <t>WERSJA 3</t>
+  </si>
+  <si>
+    <t>Rozmiar bloku 8</t>
+  </si>
+  <si>
+    <t>Rozmiar bloku 16</t>
+  </si>
+  <si>
+    <t>Rozmiar bloku 32</t>
+  </si>
 </sst>
 </file>
 
@@ -503,24 +521,3524 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 8</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$C$10:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="188278656"/>
+        <c:axId val="188280192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="188278656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188280192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="188280192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Czas [msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188278656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 8</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$C$10:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91300000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="197876352"/>
+        <c:axId val="197890816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="197876352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197890816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="197890816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Zajętość multiprocesora</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197876352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 16</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="197909120"/>
+        <c:axId val="197911296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="197909120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197911296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="197911296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Zajętość multiprocesora</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197909120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 32</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.49399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94699999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zajętość multiprocesora'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zajętość multiprocesora'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.49399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93700000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="202258304"/>
+        <c:axId val="202260480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="202258304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="202260480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="202260480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Zajętość multiprocesora</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="202258304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 16</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2000000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="183245056"/>
+        <c:axId val="183247232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="183245056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="183247232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="183247232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Czas [msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="183245056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 32</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6999999999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Czas przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Czas przetwarzania'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1000000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="188600320"/>
+        <c:axId val="188880000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="188600320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188880000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="188880000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Czas [msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188600320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 8</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$C$10:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>96.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>270.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>105.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>278.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>341.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="190031360"/>
+        <c:axId val="190033280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="190031360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="190033280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="190033280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Prędkość [Gflop/s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="190031360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 16</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>92.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>309.41000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>370.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>136.97999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>349.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>407.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="192164224"/>
+        <c:axId val="192166144"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="192164224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192166144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192166144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Prędkość [Gflop/s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192164224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 32</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>93.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>349.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>387.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prędkość przetwarzania'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Prędkość przetwarzania'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>123.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>373.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>413.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="192192512"/>
+        <c:axId val="192194432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="192192512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192194432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192194432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Prędkość [Gflop/s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192192512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 8</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$C$10:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.4185801002903137E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3405348410974227E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2969867016907183E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.4390128425164228E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3461061740822264E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.298443652302442E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="193544192"/>
+        <c:axId val="193546112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="193544192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193546112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193546112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Stopień łączenia dostępów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193544192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 16</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.7066780985043345E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5067622704105516E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.386849932193181E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.8173748372588466E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5383633058397561E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3953367336317263E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="195603840"/>
+        <c:axId val="196994560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="195603840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="196994560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="196994560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Stopień łączenia dostępów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="195603840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Rozmiar bloku</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 32</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.9989064208717394E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7071573180897945E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5068275536856748E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stopień łączenia dostępów'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WERSJA 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stopień łączenia dostępów'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.3512520101079712E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8179800550409841E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5384369800293718E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="197356160"/>
+        <c:axId val="197370624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="197356160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar macierzy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197370624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="197370624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Stopień łączenia dostępów</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="197356160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_7" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_6" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_5" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_5" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_4" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_4" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_7" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,11 +4046,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_6" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="blok8Rozmiar64_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -828,8 +4346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -905,11 +4423,11 @@
         <v>64</v>
       </c>
       <c r="F2">
-        <f>(P14+R14)/(H14+J14)</f>
+        <f t="shared" ref="F2:F10" si="0">(P14+R14)/(H14+J14)</f>
         <v>6.4185801002903137E-2</v>
       </c>
       <c r="G2">
-        <f>M14</f>
+        <f t="shared" ref="G2:G10" si="1">M14</f>
         <v>0.216</v>
       </c>
       <c r="H2">
@@ -934,15 +4452,15 @@
         <v>128</v>
       </c>
       <c r="F3">
-        <f>(P15+R15)/(H15+J15)</f>
+        <f t="shared" si="0"/>
         <v>6.3405348410974227E-2</v>
       </c>
       <c r="G3">
-        <f>M15</f>
+        <f t="shared" si="1"/>
         <v>0.84099999999999997</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="0">(Q15-T15)/Q15</f>
+        <f t="shared" ref="H3:H10" si="2">(Q15-T15)/Q15</f>
         <v>1</v>
       </c>
     </row>
@@ -960,15 +4478,15 @@
         <v>256</v>
       </c>
       <c r="F4">
-        <f>(P16+R16)/(H16+J16)</f>
+        <f t="shared" si="0"/>
         <v>6.2969867016907183E-2</v>
       </c>
       <c r="G4">
-        <f>M16</f>
+        <f t="shared" si="1"/>
         <v>0.91500000000000004</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -986,15 +4504,15 @@
         <v>64</v>
       </c>
       <c r="F5">
-        <f>(P17+R17)/(H17+J17)</f>
+        <f t="shared" si="0"/>
         <v>6.7066780985043345E-2</v>
       </c>
       <c r="G5">
-        <f>M17</f>
+        <f t="shared" si="1"/>
         <v>0.224</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1012,15 +4530,15 @@
         <v>128</v>
       </c>
       <c r="F6">
-        <f>(P18+R18)/(H18+J18)</f>
+        <f t="shared" si="0"/>
         <v>6.5067622704105516E-2</v>
       </c>
       <c r="G6">
-        <f>M18</f>
+        <f t="shared" si="1"/>
         <v>0.83899999999999997</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1038,15 +4556,15 @@
         <v>256</v>
       </c>
       <c r="F7">
-        <f>(P19+R19)/(H19+J19)</f>
+        <f t="shared" si="0"/>
         <v>6.386849932193181E-2</v>
       </c>
       <c r="G7">
-        <f>M19</f>
+        <f t="shared" si="1"/>
         <v>0.93</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1064,15 +4582,15 @@
         <v>64</v>
       </c>
       <c r="F8">
-        <f>(P20+R20)/(H20+J20)</f>
+        <f t="shared" si="0"/>
         <v>6.9989064208717394E-2</v>
       </c>
       <c r="G8">
-        <f>M20</f>
+        <f t="shared" si="1"/>
         <v>0.49399999999999999</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1090,15 +4608,15 @@
         <v>128</v>
       </c>
       <c r="F9">
-        <f>(P21+R21)/(H21+J21)</f>
+        <f t="shared" si="0"/>
         <v>6.7071573180897945E-2</v>
       </c>
       <c r="G9">
-        <f>M21</f>
+        <f t="shared" si="1"/>
         <v>0.86199999999999999</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1116,15 +4634,15 @@
         <v>256</v>
       </c>
       <c r="F10">
-        <f>(P22+R22)/(H22+J22)</f>
+        <f t="shared" si="0"/>
         <v>6.5068275536856748E-2</v>
       </c>
       <c r="G10">
-        <f>M22</f>
+        <f t="shared" si="1"/>
         <v>0.94699999999999995</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1764,7 +5282,7 @@
   <dimension ref="A4:T25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="G5" sqref="G5:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1842,7 +5360,7 @@
         <v>6.4390128425164228E-2</v>
       </c>
       <c r="G5">
-        <f>M17</f>
+        <f t="shared" ref="G5:G13" si="0">M17</f>
         <v>0.215</v>
       </c>
       <c r="H5">
@@ -1867,15 +5385,15 @@
         <v>128</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F13" si="0">(P18+R18)/(H18+J18)</f>
+        <f t="shared" ref="F6:F13" si="1">(P18+R18)/(H18+J18)</f>
         <v>6.3461061740822264E-2</v>
       </c>
       <c r="G6">
-        <f>M18</f>
+        <f t="shared" si="0"/>
         <v>0.82599999999999996</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H13" si="1">(Q18-T18)/Q18</f>
+        <f t="shared" ref="H6:H13" si="2">(Q18-T18)/Q18</f>
         <v>1</v>
       </c>
     </row>
@@ -1893,15 +5411,15 @@
         <v>256</v>
       </c>
       <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6.298443652302442E-2</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>6.298443652302442E-2</v>
-      </c>
-      <c r="G7">
-        <f>M19</f>
         <v>0.91300000000000003</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1919,15 +5437,15 @@
         <v>64</v>
       </c>
       <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.8173748372588466E-2</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>6.8173748372588466E-2</v>
-      </c>
-      <c r="G8">
-        <f>M20</f>
         <v>0.224</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1945,15 +5463,15 @@
         <v>128</v>
       </c>
       <c r="F9">
+        <f t="shared" si="1"/>
+        <v>6.5383633058397561E-2</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>6.5383633058397561E-2</v>
-      </c>
-      <c r="G9">
-        <f>M21</f>
         <v>0.84699999999999998</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1971,15 +5489,15 @@
         <v>256</v>
       </c>
       <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6.3953367336317263E-2</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>6.3953367336317263E-2</v>
-      </c>
-      <c r="G10">
-        <f>M22</f>
         <v>0.92400000000000004</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1997,15 +5515,15 @@
         <v>64</v>
       </c>
       <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7.3512520101079712E-2</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>7.3512520101079712E-2</v>
-      </c>
-      <c r="G11">
-        <f>M23</f>
         <v>0.49399999999999999</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2023,15 +5541,15 @@
         <v>128</v>
       </c>
       <c r="F12">
+        <f t="shared" si="1"/>
+        <v>6.8179800550409841E-2</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>6.8179800550409841E-2</v>
-      </c>
-      <c r="G12">
-        <f>M24</f>
         <v>0.88300000000000001</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2049,15 +5567,15 @@
         <v>256</v>
       </c>
       <c r="F13">
+        <f t="shared" si="1"/>
+        <v>6.5384369800293718E-2</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>6.5384369800293718E-2</v>
-      </c>
-      <c r="G13">
-        <f>M25</f>
         <v>0.93700000000000006</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2693,17 +6211,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B9:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
@@ -2723,12 +6240,680 @@
     <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0.124</v>
+      </c>
+      <c r="D12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D16">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E16">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D19">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D20">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E20">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B9:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>96.12</v>
+      </c>
+      <c r="D10">
+        <v>105.05</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>253.9</v>
+      </c>
+      <c r="D11">
+        <v>278.94</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>270.5</v>
+      </c>
+      <c r="D12">
+        <v>341.46</v>
+      </c>
+      <c r="E12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>92.95</v>
+      </c>
+      <c r="D14">
+        <v>136.97999999999999</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>309.41000000000003</v>
+      </c>
+      <c r="D15">
+        <v>349.44</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>370.05</v>
+      </c>
+      <c r="D16">
+        <v>407.67</v>
+      </c>
+      <c r="E16">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>93.24</v>
+      </c>
+      <c r="D18">
+        <v>123.14</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>349.9</v>
+      </c>
+      <c r="D19">
+        <v>373.03</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>387.41</v>
+      </c>
+      <c r="D20">
+        <v>413.62</v>
+      </c>
+      <c r="E20">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B9:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>6.4185801002903137E-2</v>
+      </c>
+      <c r="D10">
+        <v>6.4390128425164228E-2</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>6.3405348410974227E-2</v>
+      </c>
+      <c r="D11">
+        <v>6.3461061740822264E-2</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>6.2969867016907183E-2</v>
+      </c>
+      <c r="D12">
+        <v>6.298443652302442E-2</v>
+      </c>
+      <c r="E12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>6.7066780985043345E-2</v>
+      </c>
+      <c r="D14">
+        <v>6.8173748372588466E-2</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>6.5067622704105516E-2</v>
+      </c>
+      <c r="D15">
+        <v>6.5383633058397561E-2</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>6.386849932193181E-2</v>
+      </c>
+      <c r="D16">
+        <v>6.3953367336317263E-2</v>
+      </c>
+      <c r="E16">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>6.9989064208717394E-2</v>
+      </c>
+      <c r="D18">
+        <v>7.3512520101079712E-2</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>6.7071573180897945E-2</v>
+      </c>
+      <c r="D19">
+        <v>6.8179800550409841E-2</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>6.5068275536856748E-2</v>
+      </c>
+      <c r="D20">
+        <v>6.5384369800293718E-2</v>
+      </c>
+      <c r="E20">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B9:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>0.216</v>
+      </c>
+      <c r="D10">
+        <v>0.215</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D11">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D12">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="E12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>0.224</v>
+      </c>
+      <c r="D14">
+        <v>0.224</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="D15">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>0.93</v>
+      </c>
+      <c r="D16">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="E16">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="D20">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="E20">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>

</xml_diff>